<commit_message>
Updated test db files.
</commit_message>
<xml_diff>
--- a/tests/db/Arraignments.xlsx
+++ b/tests/db/Arraignments.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="113">
   <si>
     <t>Case</t>
   </si>
@@ -341,6 +341,18 @@
   </si>
   <si>
     <t>MICHAEL</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Moving</t>
+  </si>
+  <si>
+    <t>Non-moving</t>
+  </si>
+  <si>
+    <t>Criminal</t>
   </si>
 </sst>
 </file>
@@ -783,10 +795,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H24"/>
+  <dimension ref="A1:I24"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A11" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I24" sqref="I24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -795,7 +807,7 @@
     <col min="8" max="8" width="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -820,8 +832,11 @@
       <c r="H1" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.5">
+      <c r="I1" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
@@ -846,8 +861,11 @@
       <c r="H2" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" ht="38" x14ac:dyDescent="0.5">
+      <c r="I2" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="38" x14ac:dyDescent="0.5">
       <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
@@ -872,8 +890,11 @@
       <c r="H3" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" ht="50.7" x14ac:dyDescent="0.5">
+      <c r="I3" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="50.7" x14ac:dyDescent="0.5">
       <c r="A4" s="1" t="s">
         <v>18</v>
       </c>
@@ -898,8 +919,11 @@
       <c r="H4" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" ht="50.7" x14ac:dyDescent="0.5">
+      <c r="I4" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="50.7" x14ac:dyDescent="0.5">
       <c r="A5" s="1" t="s">
         <v>24</v>
       </c>
@@ -924,8 +948,11 @@
       <c r="H5" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" ht="25.35" x14ac:dyDescent="0.5">
+      <c r="I5" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="25.35" x14ac:dyDescent="0.5">
       <c r="A6" s="1" t="s">
         <v>29</v>
       </c>
@@ -948,8 +975,11 @@
       <c r="H6" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" ht="38" x14ac:dyDescent="0.5">
+      <c r="I6" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="38" x14ac:dyDescent="0.5">
       <c r="A7" s="1" t="s">
         <v>35</v>
       </c>
@@ -974,8 +1004,11 @@
       <c r="H7" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" ht="25.35" x14ac:dyDescent="0.5">
+      <c r="I7" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="25.35" x14ac:dyDescent="0.5">
       <c r="A8" s="1" t="s">
         <v>35</v>
       </c>
@@ -998,8 +1031,11 @@
       <c r="H8" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" ht="25.35" x14ac:dyDescent="0.5">
+      <c r="I8" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="25.35" x14ac:dyDescent="0.5">
       <c r="A9" s="1" t="s">
         <v>35</v>
       </c>
@@ -1024,8 +1060,11 @@
       <c r="H9" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" ht="38" x14ac:dyDescent="0.5">
+      <c r="I9" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="38" x14ac:dyDescent="0.5">
       <c r="A10" s="1" t="s">
         <v>47</v>
       </c>
@@ -1048,10 +1087,13 @@
         <v>17</v>
       </c>
       <c r="H10" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" ht="50.7" x14ac:dyDescent="0.5">
+        <v>100</v>
+      </c>
+      <c r="I10" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="50.7" x14ac:dyDescent="0.5">
       <c r="A11" s="1" t="s">
         <v>51</v>
       </c>
@@ -1076,8 +1118,11 @@
       <c r="H11" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" ht="50.7" x14ac:dyDescent="0.5">
+      <c r="I11" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="50.7" x14ac:dyDescent="0.5">
       <c r="A12" s="1" t="s">
         <v>58</v>
       </c>
@@ -1102,8 +1147,11 @@
       <c r="H12" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" ht="38" x14ac:dyDescent="0.5">
+      <c r="I12" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="38" x14ac:dyDescent="0.5">
       <c r="A13" s="1" t="s">
         <v>62</v>
       </c>
@@ -1128,8 +1176,11 @@
       <c r="H13" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" ht="25.35" x14ac:dyDescent="0.5">
+      <c r="I13" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="25.35" x14ac:dyDescent="0.5">
       <c r="A14" s="1" t="s">
         <v>66</v>
       </c>
@@ -1154,8 +1205,11 @@
       <c r="H14" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.5">
+      <c r="I14" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A15" s="1" t="s">
         <v>66</v>
       </c>
@@ -1180,8 +1234,11 @@
       <c r="H15" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" ht="25.35" x14ac:dyDescent="0.5">
+      <c r="I15" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="25.35" x14ac:dyDescent="0.5">
       <c r="A16" s="1" t="s">
         <v>66</v>
       </c>
@@ -1206,8 +1263,11 @@
       <c r="H16" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.5">
+      <c r="I16" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A17" s="1" t="s">
         <v>76</v>
       </c>
@@ -1232,8 +1292,11 @@
       <c r="H17" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" ht="38" x14ac:dyDescent="0.5">
+      <c r="I17" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="38" x14ac:dyDescent="0.5">
       <c r="A18" s="1" t="s">
         <v>76</v>
       </c>
@@ -1258,8 +1321,11 @@
       <c r="H18" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" ht="50.7" x14ac:dyDescent="0.5">
+      <c r="I18" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="50.7" x14ac:dyDescent="0.5">
       <c r="A19" s="1" t="s">
         <v>76</v>
       </c>
@@ -1284,8 +1350,11 @@
       <c r="H19" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="20" spans="1:8" ht="50.7" x14ac:dyDescent="0.5">
+      <c r="I19" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="50.7" x14ac:dyDescent="0.5">
       <c r="A20" s="1" t="s">
         <v>76</v>
       </c>
@@ -1310,8 +1379,11 @@
       <c r="H20" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.5">
+      <c r="I20" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A21" s="1" t="s">
         <v>89</v>
       </c>
@@ -1336,8 +1408,11 @@
       <c r="H21" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="22" spans="1:8" ht="38" x14ac:dyDescent="0.5">
+      <c r="I21" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" ht="38" x14ac:dyDescent="0.5">
       <c r="A22" s="1" t="s">
         <v>89</v>
       </c>
@@ -1362,8 +1437,11 @@
       <c r="H22" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="23" spans="1:8" ht="38" x14ac:dyDescent="0.5">
+      <c r="I22" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" ht="38" x14ac:dyDescent="0.5">
       <c r="A23" s="1" t="s">
         <v>89</v>
       </c>
@@ -1388,8 +1466,11 @@
       <c r="H23" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="24" spans="1:8" ht="23.45" customHeight="1" x14ac:dyDescent="0.5"/>
+      <c r="I23" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" ht="23.45" customHeight="1" x14ac:dyDescent="0.5"/>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="1" right="1" top="1" bottom="1" header="1" footer="1"/>

</xml_diff>

<commit_message>
Created test for database crim_sql query.
</commit_message>
<xml_diff>
--- a/tests/db/Arraignments.xlsx
+++ b/tests/db/Arraignments.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\justi\AppData\Local\Programs\Python\Python310\MuniEntry\db\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\justi\AppData\Local\Programs\Python\Python310\MuniEntry\tests\db\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3BD1C0DA-330B-44E1-B64E-69C992B38F24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B143D78B-A1AA-461D-B05D-90224FB89CA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="9015" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MuniEntryPleas" sheetId="1" r:id="rId1"/>
@@ -407,7 +407,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -425,12 +425,18 @@
       <name val="Arial"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -460,12 +466,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
   </cellXfs>
@@ -876,14 +888,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L30"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="12" width="13.73046875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:12">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -921,7 +935,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="38.25" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:12" ht="38.25">
       <c r="A2" s="1" t="s">
         <v>12</v>
       </c>
@@ -959,7 +973,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="38.25" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:12" ht="38.25">
       <c r="A3" s="1" t="s">
         <v>12</v>
       </c>
@@ -997,197 +1011,197 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="25.5" x14ac:dyDescent="0.45">
-      <c r="A4" s="1" t="s">
+    <row r="4" spans="1:12" ht="25.5">
+      <c r="A4" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D4" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="E4" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="F4" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="G4" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="H4" s="1" t="s">
+      <c r="H4" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="I4" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="J4" s="1" t="s">
+      <c r="I4" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="J4" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="K4" s="1" t="s">
+      <c r="K4" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="L4" s="1" t="s">
+      <c r="L4" s="3" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="25.5" x14ac:dyDescent="0.45">
-      <c r="A5" s="1" t="s">
+    <row r="5" spans="1:12" ht="25.5">
+      <c r="A5" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C5" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="D5" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="E5" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="F5" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="G5" s="1" t="s">
+      <c r="G5" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="H5" s="1" t="s">
+      <c r="H5" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="I5" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="J5" s="1" t="s">
+      <c r="I5" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="J5" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="K5" s="1" t="s">
+      <c r="K5" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="L5" s="1" t="s">
+      <c r="L5" s="3" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="38.25" x14ac:dyDescent="0.45">
-      <c r="A6" s="1" t="s">
+    <row r="6" spans="1:12" ht="38.25">
+      <c r="A6" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C6" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="D6" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="E6" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="F6" s="1" t="s">
+      <c r="F6" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="G6" s="1" t="s">
+      <c r="G6" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="H6" s="1" t="s">
+      <c r="H6" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="I6" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="J6" s="1" t="s">
+      <c r="I6" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="J6" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="K6" s="1" t="s">
+      <c r="K6" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="L6" s="1" t="s">
+      <c r="L6" s="3" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="38.25" x14ac:dyDescent="0.45">
-      <c r="A7" s="1" t="s">
+    <row r="7" spans="1:12" ht="38.25">
+      <c r="A7" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C7" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="D7" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="E7" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="F7" s="1" t="s">
+      <c r="F7" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="G7" s="1" t="s">
+      <c r="G7" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="H7" s="1" t="s">
+      <c r="H7" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="I7" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="J7" s="1" t="s">
+      <c r="I7" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="J7" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="K7" s="1" t="s">
+      <c r="K7" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="L7" s="1" t="s">
+      <c r="L7" s="3" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="38.25" x14ac:dyDescent="0.45">
-      <c r="A8" s="1" t="s">
+    <row r="8" spans="1:12" ht="38.25">
+      <c r="A8" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C8" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="D8" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="E8" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="F8" s="1" t="s">
+      <c r="F8" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="G8" s="1" t="s">
+      <c r="G8" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="H8" s="1" t="s">
+      <c r="H8" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="I8" s="2" t="b">
+      <c r="I8" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="J8" s="1" t="s">
+      <c r="J8" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="K8" s="1" t="s">
+      <c r="K8" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="L8" s="1" t="s">
+      <c r="L8" s="3" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="38.25" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:12" ht="38.25">
       <c r="A9" s="1" t="s">
         <v>47</v>
       </c>
@@ -1223,7 +1237,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="10" spans="1:12" ht="38.25" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:12" ht="38.25">
       <c r="A10" s="1" t="s">
         <v>52</v>
       </c>
@@ -1257,7 +1271,7 @@
       </c>
       <c r="L10" s="1"/>
     </row>
-    <row r="11" spans="1:12" ht="25.5" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:12" ht="25.5">
       <c r="A11" s="1" t="s">
         <v>59</v>
       </c>
@@ -1293,7 +1307,7 @@
       </c>
       <c r="L11" s="1"/>
     </row>
-    <row r="12" spans="1:12" ht="38.25" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:12" ht="38.25">
       <c r="A12" s="1" t="s">
         <v>59</v>
       </c>
@@ -1329,7 +1343,7 @@
       </c>
       <c r="L12" s="1"/>
     </row>
-    <row r="13" spans="1:12" ht="38.25" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:12" ht="38.25">
       <c r="A13" s="1" t="s">
         <v>59</v>
       </c>
@@ -1365,7 +1379,7 @@
       </c>
       <c r="L13" s="1"/>
     </row>
-    <row r="14" spans="1:12" ht="38.25" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:12" ht="38.25">
       <c r="A14" s="1" t="s">
         <v>59</v>
       </c>
@@ -1401,7 +1415,7 @@
       </c>
       <c r="L14" s="1"/>
     </row>
-    <row r="15" spans="1:12" ht="25.5" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:12" ht="25.5">
       <c r="A15" s="1" t="s">
         <v>70</v>
       </c>
@@ -1437,7 +1451,7 @@
       </c>
       <c r="L15" s="1"/>
     </row>
-    <row r="16" spans="1:12" ht="38.25" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:12" ht="38.25">
       <c r="A16" s="1" t="s">
         <v>70</v>
       </c>
@@ -1473,7 +1487,7 @@
       </c>
       <c r="L16" s="1"/>
     </row>
-    <row r="17" spans="1:12" ht="38.25" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:12" ht="38.25">
       <c r="A17" s="1" t="s">
         <v>70</v>
       </c>
@@ -1509,7 +1523,7 @@
       </c>
       <c r="L17" s="1"/>
     </row>
-    <row r="18" spans="1:12" ht="38.25" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:12" ht="38.25">
       <c r="A18" s="1" t="s">
         <v>70</v>
       </c>
@@ -1545,7 +1559,7 @@
       </c>
       <c r="L18" s="1"/>
     </row>
-    <row r="19" spans="1:12" ht="25.5" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:12" ht="25.5">
       <c r="A19" s="1" t="s">
         <v>84</v>
       </c>
@@ -1581,7 +1595,7 @@
       </c>
       <c r="L19" s="1"/>
     </row>
-    <row r="20" spans="1:12" ht="51" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:12" ht="51">
       <c r="A20" s="1" t="s">
         <v>84</v>
       </c>
@@ -1617,7 +1631,7 @@
       </c>
       <c r="L20" s="1"/>
     </row>
-    <row r="21" spans="1:12" ht="25.5" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:12" ht="25.5">
       <c r="A21" s="1" t="s">
         <v>84</v>
       </c>
@@ -1653,7 +1667,7 @@
       </c>
       <c r="L21" s="1"/>
     </row>
-    <row r="22" spans="1:12" ht="25.5" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:12" ht="25.5">
       <c r="A22" s="1" t="s">
         <v>96</v>
       </c>
@@ -1689,7 +1703,7 @@
       </c>
       <c r="L22" s="1"/>
     </row>
-    <row r="23" spans="1:12" ht="38.25" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:12" ht="38.25">
       <c r="A23" s="1" t="s">
         <v>96</v>
       </c>
@@ -1725,7 +1739,7 @@
       </c>
       <c r="L23" s="1"/>
     </row>
-    <row r="24" spans="1:12" ht="51" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:12" ht="51">
       <c r="A24" s="1" t="s">
         <v>101</v>
       </c>
@@ -1761,7 +1775,7 @@
       </c>
       <c r="L24" s="1"/>
     </row>
-    <row r="25" spans="1:12" ht="25.5" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:12" ht="25.5">
       <c r="A25" s="1" t="s">
         <v>101</v>
       </c>
@@ -1797,7 +1811,7 @@
       </c>
       <c r="L25" s="1"/>
     </row>
-    <row r="26" spans="1:12" ht="25.5" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:12" ht="25.5">
       <c r="A26" s="1" t="s">
         <v>109</v>
       </c>
@@ -1827,7 +1841,7 @@
       <c r="K26" s="1"/>
       <c r="L26" s="1"/>
     </row>
-    <row r="27" spans="1:12" ht="25.5" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:12" ht="25.5">
       <c r="A27" s="1" t="s">
         <v>115</v>
       </c>
@@ -1863,7 +1877,7 @@
       </c>
       <c r="L27" s="1"/>
     </row>
-    <row r="28" spans="1:12" ht="38.25" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:12" ht="38.25">
       <c r="A28" s="1" t="s">
         <v>115</v>
       </c>
@@ -1895,7 +1909,7 @@
       <c r="K28" s="1"/>
       <c r="L28" s="1"/>
     </row>
-    <row r="29" spans="1:12" ht="38.25" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:12" ht="38.25">
       <c r="A29" s="1" t="s">
         <v>115</v>
       </c>
@@ -1927,7 +1941,7 @@
       <c r="K29" s="1"/>
       <c r="L29" s="1"/>
     </row>
-    <row r="30" spans="1:12" ht="23.55" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="30" spans="1:12" ht="23.55" customHeight="1"/>
   </sheetData>
   <pageMargins left="1" right="1" top="1" bottom="1" header="1" footer="1"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>

<commit_message>
Reverted test databases to pretest data.
</commit_message>
<xml_diff>
--- a/tests/db/Arraignments.xlsx
+++ b/tests/db/Arraignments.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\justi\AppData\Local\Programs\Python\Python310\MuniEntry\tests\db\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D33BC26-101C-4802-839E-FD167C382F98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A07D44F-7485-461A-ACD1-CD1A6FEB99A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-27030" yWindow="10785" windowWidth="21600" windowHeight="11145" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="127">
   <si>
     <t>Case</t>
   </si>
@@ -401,18 +401,6 @@
   </si>
   <si>
     <t>4511.13C</t>
-  </si>
-  <si>
-    <t>12TRC1234</t>
-  </si>
-  <si>
-    <t>12TRC1234-A</t>
-  </si>
-  <si>
-    <t>TEST</t>
-  </si>
-  <si>
-    <t>MESSING</t>
   </si>
 </sst>
 </file>
@@ -898,10 +886,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L31"/>
+  <dimension ref="A1:L30"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="J2" sqref="A2:XFD2"/>
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -947,37 +935,43 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:12">
+    <row r="2" spans="1:12" ht="38.25">
       <c r="A2" s="1" t="s">
-        <v>127</v>
+        <v>12</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>128</v>
+        <v>13</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>129</v>
+        <v>14</v>
       </c>
       <c r="D2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="I2" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="K2" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="E2" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="F2" s="1">
-        <v>123.34</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="I2" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="J2" s="1"/>
-      <c r="K2" s="1"/>
-      <c r="L2" s="1"/>
+      <c r="L2" s="1" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="3" spans="1:12" ht="38.25">
       <c r="A3" s="1" t="s">
@@ -1005,7 +999,7 @@
         <v>19</v>
       </c>
       <c r="I3" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J3" s="1" t="s">
         <v>20</v>
@@ -1017,41 +1011,41 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="38.25">
-      <c r="A4" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="I4" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="J4" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="K4" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="L4" s="1" t="s">
+    <row r="4" spans="1:12" ht="25.5">
+      <c r="A4" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="I4" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="K4" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="L4" s="3" t="s">
         <v>22</v>
       </c>
     </row>
@@ -1060,7 +1054,7 @@
         <v>23</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>24</v>
+        <v>33</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>25</v>
@@ -1069,13 +1063,13 @@
         <v>26</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="H5" s="3" t="s">
         <v>30</v>
@@ -1093,12 +1087,12 @@
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="25.5">
+    <row r="6" spans="1:12" ht="38.25">
       <c r="A6" s="3" t="s">
         <v>23</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>25</v>
@@ -1107,13 +1101,13 @@
         <v>26</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="H6" s="3" t="s">
         <v>30</v>
@@ -1136,7 +1130,7 @@
         <v>23</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>25</v>
@@ -1145,10 +1139,10 @@
         <v>26</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="G7" s="3" t="s">
         <v>40</v>
@@ -1174,7 +1168,7 @@
         <v>23</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>25</v>
@@ -1183,19 +1177,19 @@
         <v>26</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="H8" s="3" t="s">
         <v>30</v>
       </c>
       <c r="I8" s="4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J8" s="3" t="s">
         <v>31</v>
@@ -1208,104 +1202,102 @@
       </c>
     </row>
     <row r="9" spans="1:12" ht="38.25">
-      <c r="A9" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="F9" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="G9" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="H9" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="I9" s="4" t="b">
+      <c r="A9" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="H9" s="1"/>
+      <c r="I9" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="J9" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="K9" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="L9" s="3" t="s">
+      <c r="J9" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="L9" s="1" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="10" spans="1:12" ht="38.25">
       <c r="A10" s="1" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>14</v>
+        <v>54</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>15</v>
+        <v>55</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>49</v>
+        <v>56</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="H10" s="1"/>
       <c r="I10" s="2" t="b">
         <v>0</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>20</v>
+        <v>58</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="L10" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" ht="38.25">
+        <v>26</v>
+      </c>
+      <c r="L10" s="1"/>
+    </row>
+    <row r="11" spans="1:12" ht="25.5">
       <c r="A11" s="1" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>54</v>
+        <v>61</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>55</v>
+        <v>62</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>56</v>
+        <v>63</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="H11" s="1"/>
+        <v>36</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>19</v>
+      </c>
       <c r="I11" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J11" s="1" t="s">
         <v>58</v>
@@ -1315,12 +1307,12 @@
       </c>
       <c r="L11" s="1"/>
     </row>
-    <row r="12" spans="1:12" ht="25.5">
+    <row r="12" spans="1:12" ht="38.25">
       <c r="A12" s="1" t="s">
         <v>59</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>61</v>
@@ -1329,10 +1321,10 @@
         <v>62</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="G12" s="1" t="s">
         <v>36</v>
@@ -1356,7 +1348,7 @@
         <v>59</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>61</v>
@@ -1365,13 +1357,13 @@
         <v>62</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>66</v>
+        <v>38</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>67</v>
+        <v>39</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="H13" s="1" t="s">
         <v>19</v>
@@ -1392,7 +1384,7 @@
         <v>59</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>61</v>
@@ -1401,19 +1393,19 @@
         <v>62</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="H14" s="1" t="s">
         <v>19</v>
       </c>
       <c r="I14" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J14" s="1" t="s">
         <v>58</v>
@@ -1423,48 +1415,48 @@
       </c>
       <c r="L14" s="1"/>
     </row>
-    <row r="15" spans="1:12" ht="38.25">
+    <row r="15" spans="1:12" ht="25.5">
       <c r="A15" s="1" t="s">
-        <v>59</v>
+        <v>70</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>61</v>
+        <v>72</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>62</v>
+        <v>73</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>45</v>
+        <v>27</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>46</v>
+        <v>28</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>19</v>
+        <v>74</v>
       </c>
       <c r="I15" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>58</v>
+        <v>75</v>
       </c>
       <c r="K15" s="1" t="s">
-        <v>26</v>
+        <v>76</v>
       </c>
       <c r="L15" s="1"/>
     </row>
-    <row r="16" spans="1:12" ht="25.5">
+    <row r="16" spans="1:12" ht="38.25">
       <c r="A16" s="1" t="s">
         <v>70</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>71</v>
+        <v>77</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>72</v>
@@ -1473,10 +1465,10 @@
         <v>73</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>27</v>
+        <v>78</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>28</v>
+        <v>79</v>
       </c>
       <c r="G16" s="1" t="s">
         <v>29</v>
@@ -1500,7 +1492,7 @@
         <v>70</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>72</v>
@@ -1509,13 +1501,13 @@
         <v>73</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>29</v>
+        <v>40</v>
       </c>
       <c r="H17" s="1" t="s">
         <v>74</v>
@@ -1536,7 +1528,7 @@
         <v>70</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>72</v>
@@ -1545,10 +1537,10 @@
         <v>73</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>81</v>
+        <v>38</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>82</v>
+        <v>39</v>
       </c>
       <c r="G18" s="1" t="s">
         <v>40</v>
@@ -1567,27 +1559,27 @@
       </c>
       <c r="L18" s="1"/>
     </row>
-    <row r="19" spans="1:12" ht="38.25">
+    <row r="19" spans="1:12" ht="25.5">
       <c r="A19" s="1" t="s">
-        <v>70</v>
+        <v>84</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>72</v>
+        <v>86</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>73</v>
+        <v>87</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>39</v>
+        <v>28</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>40</v>
+        <v>29</v>
       </c>
       <c r="H19" s="1" t="s">
         <v>74</v>
@@ -1596,19 +1588,19 @@
         <v>1</v>
       </c>
       <c r="J19" s="1" t="s">
-        <v>75</v>
+        <v>88</v>
       </c>
       <c r="K19" s="1" t="s">
-        <v>76</v>
+        <v>89</v>
       </c>
       <c r="L19" s="1"/>
     </row>
-    <row r="20" spans="1:12" ht="25.5">
+    <row r="20" spans="1:12" ht="51">
       <c r="A20" s="1" t="s">
         <v>84</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>86</v>
@@ -1617,10 +1609,10 @@
         <v>87</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>27</v>
+        <v>91</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>28</v>
+        <v>92</v>
       </c>
       <c r="G20" s="1" t="s">
         <v>29</v>
@@ -1639,12 +1631,12 @@
       </c>
       <c r="L20" s="1"/>
     </row>
-    <row r="21" spans="1:12" ht="51">
+    <row r="21" spans="1:12" ht="25.5">
       <c r="A21" s="1" t="s">
         <v>84</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>86</v>
@@ -1653,13 +1645,13 @@
         <v>87</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>29</v>
+        <v>40</v>
       </c>
       <c r="H21" s="1" t="s">
         <v>74</v>
@@ -1677,25 +1669,25 @@
     </row>
     <row r="22" spans="1:12" ht="25.5">
       <c r="A22" s="1" t="s">
-        <v>84</v>
+        <v>96</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>86</v>
+        <v>98</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>87</v>
+        <v>99</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>94</v>
+        <v>27</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>95</v>
+        <v>28</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>40</v>
+        <v>29</v>
       </c>
       <c r="H22" s="1" t="s">
         <v>74</v>
@@ -1704,19 +1696,19 @@
         <v>1</v>
       </c>
       <c r="J22" s="1" t="s">
-        <v>88</v>
+        <v>58</v>
       </c>
       <c r="K22" s="1" t="s">
-        <v>89</v>
+        <v>26</v>
       </c>
       <c r="L22" s="1"/>
     </row>
-    <row r="23" spans="1:12" ht="25.5">
+    <row r="23" spans="1:12" ht="38.25">
       <c r="A23" s="1" t="s">
         <v>96</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>98</v>
@@ -1725,13 +1717,13 @@
         <v>99</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>27</v>
+        <v>81</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>28</v>
+        <v>82</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>29</v>
+        <v>40</v>
       </c>
       <c r="H23" s="1" t="s">
         <v>74</v>
@@ -1747,27 +1739,27 @@
       </c>
       <c r="L23" s="1"/>
     </row>
-    <row r="24" spans="1:12" ht="38.25">
+    <row r="24" spans="1:12" ht="51">
       <c r="A24" s="1" t="s">
-        <v>96</v>
+        <v>101</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>98</v>
+        <v>103</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>99</v>
+        <v>104</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>81</v>
+        <v>91</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>82</v>
+        <v>92</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>40</v>
+        <v>29</v>
       </c>
       <c r="H24" s="1" t="s">
         <v>74</v>
@@ -1776,19 +1768,19 @@
         <v>1</v>
       </c>
       <c r="J24" s="1" t="s">
-        <v>58</v>
+        <v>105</v>
       </c>
       <c r="K24" s="1" t="s">
-        <v>26</v>
+        <v>106</v>
       </c>
       <c r="L24" s="1"/>
     </row>
-    <row r="25" spans="1:12" ht="51">
+    <row r="25" spans="1:12" ht="25.5">
       <c r="A25" s="1" t="s">
         <v>101</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>102</v>
+        <v>107</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>103</v>
@@ -1797,13 +1789,13 @@
         <v>104</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>91</v>
+        <v>108</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>29</v>
+        <v>40</v>
       </c>
       <c r="H25" s="1" t="s">
         <v>74</v>
@@ -1821,76 +1813,76 @@
     </row>
     <row r="26" spans="1:12" ht="25.5">
       <c r="A26" s="1" t="s">
-        <v>101</v>
+        <v>109</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>103</v>
+        <v>111</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>104</v>
+        <v>112</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>108</v>
+        <v>113</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="G26" s="1" t="s">
-        <v>40</v>
-      </c>
+        <v>114</v>
+      </c>
+      <c r="G26" s="1"/>
       <c r="H26" s="1" t="s">
-        <v>74</v>
+        <v>30</v>
       </c>
       <c r="I26" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="J26" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="K26" s="1" t="s">
-        <v>106</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="J26" s="1"/>
+      <c r="K26" s="1"/>
       <c r="L26" s="1"/>
     </row>
     <row r="27" spans="1:12" ht="25.5">
       <c r="A27" s="1" t="s">
-        <v>109</v>
+        <v>115</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>110</v>
+        <v>116</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>111</v>
+        <v>117</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>112</v>
+        <v>118</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>113</v>
+        <v>27</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="G27" s="1"/>
+        <v>28</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>29</v>
+      </c>
       <c r="H27" s="1" t="s">
-        <v>30</v>
+        <v>74</v>
       </c>
       <c r="I27" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="J27" s="1"/>
-      <c r="K27" s="1"/>
+        <v>1</v>
+      </c>
+      <c r="J27" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="K27" s="1" t="s">
+        <v>120</v>
+      </c>
       <c r="L27" s="1"/>
     </row>
-    <row r="28" spans="1:12" ht="25.5">
+    <row r="28" spans="1:12" ht="38.25">
       <c r="A28" s="1" t="s">
         <v>115</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>116</v>
+        <v>121</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>117</v>
@@ -1899,10 +1891,10 @@
         <v>118</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>27</v>
+        <v>122</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>28</v>
+        <v>123</v>
       </c>
       <c r="G28" s="1" t="s">
         <v>29</v>
@@ -1913,12 +1905,8 @@
       <c r="I28" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="J28" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="K28" s="1" t="s">
-        <v>120</v>
-      </c>
+      <c r="J28" s="1"/>
+      <c r="K28" s="1"/>
       <c r="L28" s="1"/>
     </row>
     <row r="29" spans="1:12" ht="38.25">
@@ -1926,7 +1914,7 @@
         <v>115</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>117</v>
@@ -1935,13 +1923,13 @@
         <v>118</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>29</v>
+        <v>40</v>
       </c>
       <c r="H29" s="1" t="s">
         <v>74</v>
@@ -1953,39 +1941,7 @@
       <c r="K29" s="1"/>
       <c r="L29" s="1"/>
     </row>
-    <row r="30" spans="1:12" ht="38.25">
-      <c r="A30" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="D30" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="E30" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="F30" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="G30" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="H30" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="I30" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="J30" s="1"/>
-      <c r="K30" s="1"/>
-      <c r="L30" s="1"/>
-    </row>
-    <row r="31" spans="1:12" ht="23.55" customHeight="1"/>
+    <row r="30" spans="1:12" ht="23.55" customHeight="1"/>
   </sheetData>
   <pageMargins left="1" right="1" top="1" bottom="1" header="1" footer="1"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>

<commit_message>
Fixed insert_daily_case_list_sql_data and sql_query for it.
</commit_message>
<xml_diff>
--- a/tests/db/Arraignments.xlsx
+++ b/tests/db/Arraignments.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25128"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\justi\AppData\Local\Programs\Python\Python310\MuniEntry\tests\db\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A07D44F-7485-461A-ACD1-CD1A6FEB99A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{726323BF-BFC3-4A71-B5D7-D5F1E9E1DB86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-27030" yWindow="10785" windowWidth="21600" windowHeight="11145" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="47532" yWindow="8304" windowWidth="21588" windowHeight="11136" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MuniEntryPleas" sheetId="1" r:id="rId1"/>
@@ -184,9 +184,6 @@
     <t>21CRB01597-A</t>
   </si>
   <si>
-    <t>ANSLEY</t>
-  </si>
-  <si>
     <t>JACOB</t>
   </si>
   <si>
@@ -401,6 +398,9 @@
   </si>
   <si>
     <t>4511.13C</t>
+  </si>
+  <si>
+    <t>O'REILLY</t>
   </si>
 </sst>
 </file>
@@ -888,8 +888,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L30"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -1245,16 +1245,16 @@
         <v>53</v>
       </c>
       <c r="C10" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="D10" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="E10" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="E10" s="1" t="s">
+      <c r="F10" s="1" t="s">
         <v>56</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>57</v>
       </c>
       <c r="G10" s="1" t="s">
         <v>40</v>
@@ -1264,7 +1264,7 @@
         <v>0</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="K10" s="1" t="s">
         <v>26</v>
@@ -1273,22 +1273,22 @@
     </row>
     <row r="11" spans="1:12" ht="25.5">
       <c r="A11" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="C11" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="D11" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="E11" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="E11" s="1" t="s">
+      <c r="F11" s="1" t="s">
         <v>63</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>64</v>
       </c>
       <c r="G11" s="1" t="s">
         <v>36</v>
@@ -1300,7 +1300,7 @@
         <v>1</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="K11" s="1" t="s">
         <v>26</v>
@@ -1309,22 +1309,22 @@
     </row>
     <row r="12" spans="1:12" ht="38.25">
       <c r="A12" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B12" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="E12" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="C12" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="E12" s="1" t="s">
+      <c r="F12" s="1" t="s">
         <v>66</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>67</v>
       </c>
       <c r="G12" s="1" t="s">
         <v>36</v>
@@ -1336,7 +1336,7 @@
         <v>1</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="K12" s="1" t="s">
         <v>26</v>
@@ -1345,16 +1345,16 @@
     </row>
     <row r="13" spans="1:12" ht="38.25">
       <c r="A13" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C13" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D13" s="1" t="s">
         <v>61</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>62</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>38</v>
@@ -1372,7 +1372,7 @@
         <v>1</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="K13" s="1" t="s">
         <v>26</v>
@@ -1381,16 +1381,16 @@
     </row>
     <row r="14" spans="1:12" ht="38.25">
       <c r="A14" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C14" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D14" s="1" t="s">
         <v>61</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>62</v>
       </c>
       <c r="E14" s="1" t="s">
         <v>45</v>
@@ -1408,7 +1408,7 @@
         <v>0</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="K14" s="1" t="s">
         <v>26</v>
@@ -1417,16 +1417,16 @@
     </row>
     <row r="15" spans="1:12" ht="25.5">
       <c r="A15" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B15" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="C15" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="C15" s="1" t="s">
+      <c r="D15" s="1" t="s">
         <v>72</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>73</v>
       </c>
       <c r="E15" s="1" t="s">
         <v>27</v>
@@ -1438,103 +1438,103 @@
         <v>29</v>
       </c>
       <c r="H15" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="I15" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="J15" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="I15" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="J15" s="1" t="s">
+      <c r="K15" s="1" t="s">
         <v>75</v>
-      </c>
-      <c r="K15" s="1" t="s">
-        <v>76</v>
       </c>
       <c r="L15" s="1"/>
     </row>
     <row r="16" spans="1:12" ht="38.25">
       <c r="A16" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B16" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="E16" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="C16" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="E16" s="1" t="s">
+      <c r="F16" s="1" t="s">
         <v>78</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>79</v>
       </c>
       <c r="G16" s="1" t="s">
         <v>29</v>
       </c>
       <c r="H16" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="I16" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="J16" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="I16" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="J16" s="1" t="s">
+      <c r="K16" s="1" t="s">
         <v>75</v>
-      </c>
-      <c r="K16" s="1" t="s">
-        <v>76</v>
       </c>
       <c r="L16" s="1"/>
     </row>
     <row r="17" spans="1:12" ht="38.25">
       <c r="A17" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B17" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="E17" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="C17" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="E17" s="1" t="s">
+      <c r="F17" s="1" t="s">
         <v>81</v>
-      </c>
-      <c r="F17" s="1" t="s">
-        <v>82</v>
       </c>
       <c r="G17" s="1" t="s">
         <v>40</v>
       </c>
       <c r="H17" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="I17" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="J17" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="I17" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="J17" s="1" t="s">
+      <c r="K17" s="1" t="s">
         <v>75</v>
-      </c>
-      <c r="K17" s="1" t="s">
-        <v>76</v>
       </c>
       <c r="L17" s="1"/>
     </row>
     <row r="18" spans="1:12" ht="38.25">
       <c r="A18" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C18" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D18" s="1" t="s">
         <v>72</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>73</v>
       </c>
       <c r="E18" s="1" t="s">
         <v>38</v>
@@ -1546,31 +1546,31 @@
         <v>40</v>
       </c>
       <c r="H18" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="I18" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="J18" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="I18" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="J18" s="1" t="s">
+      <c r="K18" s="1" t="s">
         <v>75</v>
-      </c>
-      <c r="K18" s="1" t="s">
-        <v>76</v>
       </c>
       <c r="L18" s="1"/>
     </row>
     <row r="19" spans="1:12" ht="25.5">
       <c r="A19" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B19" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="C19" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="C19" s="1" t="s">
+      <c r="D19" s="1" t="s">
         <v>86</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>87</v>
       </c>
       <c r="E19" s="1" t="s">
         <v>27</v>
@@ -1582,103 +1582,103 @@
         <v>29</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I19" s="2" t="b">
         <v>1</v>
       </c>
       <c r="J19" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="K19" s="1" t="s">
         <v>88</v>
-      </c>
-      <c r="K19" s="1" t="s">
-        <v>89</v>
       </c>
       <c r="L19" s="1"/>
     </row>
     <row r="20" spans="1:12" ht="51">
       <c r="A20" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B20" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="E20" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="C20" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="E20" s="1" t="s">
+      <c r="F20" s="1" t="s">
         <v>91</v>
-      </c>
-      <c r="F20" s="1" t="s">
-        <v>92</v>
       </c>
       <c r="G20" s="1" t="s">
         <v>29</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I20" s="2" t="b">
         <v>1</v>
       </c>
       <c r="J20" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="K20" s="1" t="s">
         <v>88</v>
-      </c>
-      <c r="K20" s="1" t="s">
-        <v>89</v>
       </c>
       <c r="L20" s="1"/>
     </row>
     <row r="21" spans="1:12" ht="25.5">
       <c r="A21" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B21" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="E21" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="C21" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="E21" s="1" t="s">
+      <c r="F21" s="1" t="s">
         <v>94</v>
-      </c>
-      <c r="F21" s="1" t="s">
-        <v>95</v>
       </c>
       <c r="G21" s="1" t="s">
         <v>40</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I21" s="2" t="b">
         <v>1</v>
       </c>
       <c r="J21" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="K21" s="1" t="s">
         <v>88</v>
-      </c>
-      <c r="K21" s="1" t="s">
-        <v>89</v>
       </c>
       <c r="L21" s="1"/>
     </row>
     <row r="22" spans="1:12" ht="25.5">
       <c r="A22" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B22" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="B22" s="1" t="s">
+      <c r="C22" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="C22" s="1" t="s">
+      <c r="D22" s="1" t="s">
         <v>98</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>99</v>
       </c>
       <c r="E22" s="1" t="s">
         <v>27</v>
@@ -1690,13 +1690,13 @@
         <v>29</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I22" s="2" t="b">
         <v>1</v>
       </c>
       <c r="J22" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="K22" s="1" t="s">
         <v>26</v>
@@ -1705,34 +1705,34 @@
     </row>
     <row r="23" spans="1:12" ht="38.25">
       <c r="A23" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C23" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="D23" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="D23" s="1" t="s">
-        <v>99</v>
-      </c>
       <c r="E23" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="F23" s="1" t="s">
         <v>81</v>
-      </c>
-      <c r="F23" s="1" t="s">
-        <v>82</v>
       </c>
       <c r="G23" s="1" t="s">
         <v>40</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I23" s="2" t="b">
         <v>1</v>
       </c>
       <c r="J23" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="K23" s="1" t="s">
         <v>26</v>
@@ -1741,94 +1741,94 @@
     </row>
     <row r="24" spans="1:12" ht="51">
       <c r="A24" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B24" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="B24" s="1" t="s">
+      <c r="C24" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="C24" s="1" t="s">
+      <c r="D24" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="D24" s="1" t="s">
-        <v>104</v>
-      </c>
       <c r="E24" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="F24" s="1" t="s">
         <v>91</v>
-      </c>
-      <c r="F24" s="1" t="s">
-        <v>92</v>
       </c>
       <c r="G24" s="1" t="s">
         <v>29</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I24" s="2" t="b">
         <v>1</v>
       </c>
       <c r="J24" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="K24" s="1" t="s">
         <v>105</v>
-      </c>
-      <c r="K24" s="1" t="s">
-        <v>106</v>
       </c>
       <c r="L24" s="1"/>
     </row>
     <row r="25" spans="1:12" ht="25.5">
       <c r="A25" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B25" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="E25" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="C25" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="D25" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="E25" s="1" t="s">
-        <v>108</v>
-      </c>
       <c r="F25" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G25" s="1" t="s">
         <v>40</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I25" s="2" t="b">
         <v>1</v>
       </c>
       <c r="J25" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="K25" s="1" t="s">
         <v>105</v>
-      </c>
-      <c r="K25" s="1" t="s">
-        <v>106</v>
       </c>
       <c r="L25" s="1"/>
     </row>
     <row r="26" spans="1:12" ht="25.5">
       <c r="A26" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B26" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="B26" s="1" t="s">
+      <c r="C26" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="C26" s="1" t="s">
+      <c r="D26" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="D26" s="1" t="s">
+      <c r="E26" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="E26" s="1" t="s">
+      <c r="F26" s="1" t="s">
         <v>113</v>
-      </c>
-      <c r="F26" s="1" t="s">
-        <v>114</v>
       </c>
       <c r="G26" s="1"/>
       <c r="H26" s="1" t="s">
@@ -1843,16 +1843,16 @@
     </row>
     <row r="27" spans="1:12" ht="25.5">
       <c r="A27" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="B27" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="B27" s="1" t="s">
+      <c r="C27" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="C27" s="1" t="s">
+      <c r="D27" s="1" t="s">
         <v>117</v>
-      </c>
-      <c r="D27" s="1" t="s">
-        <v>118</v>
       </c>
       <c r="E27" s="1" t="s">
         <v>27</v>
@@ -1864,43 +1864,43 @@
         <v>29</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I27" s="2" t="b">
         <v>1</v>
       </c>
       <c r="J27" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="K27" s="1" t="s">
         <v>119</v>
-      </c>
-      <c r="K27" s="1" t="s">
-        <v>120</v>
       </c>
       <c r="L27" s="1"/>
     </row>
     <row r="28" spans="1:12" ht="38.25">
       <c r="A28" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B28" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="E28" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="C28" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="D28" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="E28" s="1" t="s">
+      <c r="F28" s="1" t="s">
         <v>122</v>
-      </c>
-      <c r="F28" s="1" t="s">
-        <v>123</v>
       </c>
       <c r="G28" s="1" t="s">
         <v>29</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I28" s="2" t="b">
         <v>1</v>
@@ -1911,28 +1911,28 @@
     </row>
     <row r="29" spans="1:12" ht="38.25">
       <c r="A29" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B29" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="E29" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="C29" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="D29" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="E29" s="1" t="s">
+      <c r="F29" s="1" t="s">
         <v>125</v>
-      </c>
-      <c r="F29" s="1" t="s">
-        <v>126</v>
       </c>
       <c r="G29" s="1" t="s">
         <v>40</v>
       </c>
       <c r="H29" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I29" s="2" t="b">
         <v>1</v>

</xml_diff>